<commit_message>
add check Vert and Horiz; fist ver. gen. BG
</commit_message>
<xml_diff>
--- a/ExampleOfBG.xlsx
+++ b/ExampleOfBG.xlsx
@@ -23,8 +23,68 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Пользователь Windows</author>
+  </authors>
+  <commentList>
+    <comment ref="B12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Sznv91:
+8 - длинна поля
+2 - позиция сгенерированного числа
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="7"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Sznv:
+Определение разрешенной длины:
+длинна корабля - 1(1=сгенерировання ячейка)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Sznv:
+3 - заданная длинна корабля
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>A0</t>
   </si>
@@ -216,13 +276,94 @@
   </si>
   <si>
     <t>H7</t>
+  </si>
+  <si>
+    <t>6+2=8</t>
+  </si>
+  <si>
+    <t>Больше чем длинна поля</t>
+  </si>
+  <si>
+    <t>8-2=6</t>
+  </si>
+  <si>
+    <t>6+3=9</t>
+  </si>
+  <si>
+    <t>(8-1)-1=6</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>(8-1)-2=5</t>
+  </si>
+  <si>
+    <t>5+3=8</t>
+  </si>
+  <si>
+    <t>8=8</t>
+  </si>
+  <si>
+    <t>ok left</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>(8-1)-3=4</t>
+  </si>
+  <si>
+    <t>4+3=7</t>
+  </si>
+  <si>
+    <t>7&lt;8</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>9&gt;8</t>
+  </si>
+  <si>
+    <t>fault left</t>
+  </si>
+  <si>
+    <t>(8-1)-2+3</t>
+  </si>
+  <si>
+    <t>(8-1)-6=1</t>
+  </si>
+  <si>
+    <t>Одна ячейка осталсь справа. Не влезет корабль из 3х ячеек</t>
+  </si>
+  <si>
+    <t>Right fall</t>
+  </si>
+  <si>
+    <t>(3-1)&gt;1</t>
+  </si>
+  <si>
+    <t>1 - первая сгенерированная ячейка</t>
+  </si>
+  <si>
+    <t>(8-1)-5=2</t>
+  </si>
+  <si>
+    <t>(3-1)=2</t>
+  </si>
+  <si>
+    <t>Все ок, такой корабль пролезет</t>
+  </si>
+  <si>
+    <t>7-6=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +371,21 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -246,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -254,14 +410,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -541,11 +786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,239 +798,387 @@
     <col min="1" max="8" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>63</v>
       </c>
       <c r="J1">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="J2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="7" t="s">
         <v>48</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="11" t="s">
         <v>55</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add check crossfire cells; need fix problems
</commit_message>
<xml_diff>
--- a/ExampleOfBG.xlsx
+++ b/ExampleOfBG.xlsx
@@ -402,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -431,17 +431,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -457,17 +446,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -490,23 +468,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -790,7 +806,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,13 +818,13 @@
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -820,7 +836,7 @@
       <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J1">
@@ -828,28 +844,28 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J2">
@@ -857,28 +873,28 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J3">
@@ -886,28 +902,28 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="J4">
@@ -915,28 +931,28 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="J5">
@@ -944,28 +960,28 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="J6">
@@ -973,28 +989,28 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>48</v>
       </c>
       <c r="J7">
@@ -1002,28 +1018,28 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>55</v>
       </c>
       <c r="J8">

</xml_diff>